<commit_message>
Updated YouTube video link
</commit_message>
<xml_diff>
--- a/Generic dependent drop-down template/Example using SumProduct_November_2018_Final_Friday_Fix.xlsx
+++ b/Generic dependent drop-down template/Example using SumProduct_November_2018_Final_Friday_Fix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\devel\GitHub\r_excel-stuff\Generic dependent drop-down template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A06C5BB2-811A-411D-BC8D-EB2A24AF887F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B37F94B4-A5A3-4633-B93B-C657D1141C01}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" tabRatio="695" activeTab="8" xr2:uid="{CFE9C8BB-2459-420C-9738-69DA0FE3A2B5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" tabRatio="695" xr2:uid="{CFE9C8BB-2459-420C-9738-69DA0FE3A2B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="7" r:id="rId1"/>
@@ -1440,7 +1440,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> See demo at: &lt;update needed&gt;</a:t>
+            <a:t> See demo at https://youtu.be/FFWmlDRkHwc</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2367,7 +2367,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{75872AE6-FE3C-45DF-BE3D-C69B6BA08C67}" name="Level_2" displayName="Level_2" ref="A1:B4" tableType="queryTable" totalsRowShown="0" headerRowCellStyle="Comma">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{75872AE6-FE3C-45DF-BE3D-C69B6BA08C67}" name="Level_2" displayName="Level_2" ref="A1:B4" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:B4" xr:uid="{65D9AE05-491D-4CA4-A821-931069DDA99A}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{73DCFD1E-A4BE-4FB7-9FD8-A38ABD6D09C9}" uniqueName="1" name="Toyota" queryTableFieldId="4"/>
@@ -2885,7 +2885,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -6265,7 +6265,7 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:FE1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+    <sheetView topLeftCell="M1" workbookViewId="0">
       <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>

</xml_diff>